<commit_message>
Add cloud deployment: Neon PostgreSQL, Railway config, scraper automation
</commit_message>
<xml_diff>
--- a/CATI/saved_states/NABIL_future_30_day_forecast.xlsx
+++ b/CATI/saved_states/NABIL_future_30_day_forecast.xlsx
@@ -464,7 +464,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.5714081285771611</v>
+        <v>0.5885267759242613</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.5711269543859615</v>
+        <v>0.5911887232155837</v>
       </c>
     </row>
     <row r="4">
@@ -490,7 +490,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.5789961472963068</v>
+        <v>0.6023564448209522</v>
       </c>
     </row>
     <row r="5">
@@ -503,7 +503,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.5833010320224723</v>
+        <v>0.6108945781989429</v>
       </c>
     </row>
     <row r="6">
@@ -516,7 +516,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.5879504372194981</v>
+        <v>0.6198713159374452</v>
       </c>
     </row>
     <row r="7">
@@ -529,7 +529,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.590979417611557</v>
+        <v>0.6258634400603158</v>
       </c>
     </row>
     <row r="8">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.5945961374357285</v>
+        <v>0.6316463320625886</v>
       </c>
     </row>
     <row r="9">
@@ -555,7 +555,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.5911753421389493</v>
+        <v>0.6319819224597421</v>
       </c>
     </row>
     <row r="10">
@@ -568,7 +568,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.5975807797608076</v>
+        <v>0.6414839479224961</v>
       </c>
     </row>
     <row r="11">
@@ -581,7 +581,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.6008740195909528</v>
+        <v>0.647225296788371</v>
       </c>
     </row>
     <row r="12">
@@ -594,7 +594,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.6022074941648256</v>
+        <v>0.6508056056512515</v>
       </c>
     </row>
     <row r="13">
@@ -607,7 +607,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.6014530421058046</v>
+        <v>0.6519278257512676</v>
       </c>
     </row>
     <row r="14">
@@ -620,7 +620,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.5959883727740045</v>
+        <v>0.6475786384791731</v>
       </c>
     </row>
     <row r="15">
@@ -633,7 +633,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.5994333289469029</v>
+        <v>0.6510664671705201</v>
       </c>
     </row>
     <row r="16">
@@ -646,7 +646,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.6003160695788545</v>
+        <v>0.6512044973111157</v>
       </c>
     </row>
     <row r="17">
@@ -659,7 +659,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.6064931255528676</v>
+        <v>0.6549080893090113</v>
       </c>
     </row>
     <row r="18">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.6004546891820318</v>
+        <v>0.6454641940248406</v>
       </c>
     </row>
     <row r="19">
@@ -685,7 +685,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.5962182832485803</v>
+        <v>0.6373885823827905</v>
       </c>
     </row>
     <row r="20">
@@ -698,7 +698,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.5979863728149064</v>
+        <v>0.6372392867940888</v>
       </c>
     </row>
     <row r="21">
@@ -711,7 +711,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.6013956810328778</v>
+        <v>0.640971269853901</v>
       </c>
     </row>
     <row r="22">
@@ -724,7 +724,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.60133975110494</v>
+        <v>0.6431045510590538</v>
       </c>
     </row>
     <row r="23">
@@ -737,7 +737,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.5978810480428727</v>
+        <v>0.6404464194889945</v>
       </c>
     </row>
     <row r="24">
@@ -750,7 +750,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.5939538514825187</v>
+        <v>0.6359716520654831</v>
       </c>
     </row>
     <row r="25">
@@ -763,7 +763,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.5828670133827567</v>
+        <v>0.6260983226885014</v>
       </c>
     </row>
     <row r="26">
@@ -776,7 +776,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.5758080406683472</v>
+        <v>0.6197587140540662</v>
       </c>
     </row>
     <row r="27">
@@ -789,7 +789,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.5761492939507517</v>
+        <v>0.6170677713373381</v>
       </c>
     </row>
     <row r="28">
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.5756633828189088</v>
+        <v>0.6185438885960699</v>
       </c>
     </row>
     <row r="29">
@@ -815,7 +815,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.5755761916845268</v>
+        <v>0.6193557328281218</v>
       </c>
     </row>
     <row r="30">
@@ -828,7 +828,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.5757183124037188</v>
+        <v>0.6195280367346949</v>
       </c>
     </row>
     <row r="31">
@@ -841,7 +841,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.5759209940936281</v>
+        <v>0.6197502568040014</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix pipeline, clean CSVs, and restrict to 6 stocks
</commit_message>
<xml_diff>
--- a/CATI/saved_states/NABIL_future_30_day_forecast.xlsx
+++ b/CATI/saved_states/NABIL_future_30_day_forecast.xlsx
@@ -456,392 +456,392 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45938</v>
+        <v>45940</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.5885267759242613</v>
+        <v>0.1285659813084559</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45939</v>
+        <v>45943</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.5911887232155837</v>
+        <v>0.1287382036470091</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45940</v>
+        <v>45944</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.6023564448209522</v>
+        <v>0.1291497737191831</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45943</v>
+        <v>45945</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.6108945781989429</v>
+        <v>0.1291170805715238</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45944</v>
+        <v>45946</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.6198713159374452</v>
+        <v>0.1306651375941179</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45945</v>
+        <v>45947</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.6258634400603158</v>
+        <v>0.1304588459185503</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45946</v>
+        <v>45950</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.6316463320625886</v>
+        <v>0.1314351016396507</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45947</v>
+        <v>45951</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.6319819224597421</v>
+        <v>0.1328840659403057</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45950</v>
+        <v>45952</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.6414839479224961</v>
+        <v>0.1349019262052822</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45951</v>
+        <v>45953</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.647225296788371</v>
+        <v>0.1334518656093679</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45952</v>
+        <v>45954</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.6508056056512515</v>
+        <v>0.1335783168632589</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45953</v>
+        <v>45957</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.6519278257512676</v>
+        <v>0.1334961743382388</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45954</v>
+        <v>45958</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.6475786384791731</v>
+        <v>0.1335629687932902</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45957</v>
+        <v>45959</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.6510664671705201</v>
+        <v>0.1323912033437438</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45958</v>
+        <v>45960</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.6512044973111157</v>
+        <v>0.1325974801181503</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45959</v>
+        <v>45961</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.6549080893090113</v>
+        <v>0.1303342813790535</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45960</v>
+        <v>45964</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.6454641940248406</v>
+        <v>0.1304443786085342</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45961</v>
+        <v>45965</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.6373885823827905</v>
+        <v>0.1306046554983352</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45964</v>
+        <v>45966</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.6372392867940888</v>
+        <v>0.1309971520841812</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45965</v>
+        <v>45967</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.640971269853901</v>
+        <v>0.1318909451504794</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45966</v>
+        <v>45968</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.6431045510590538</v>
+        <v>0.131755389287099</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45967</v>
+        <v>45971</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.6404464194889945</v>
+        <v>0.1317243901480579</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45968</v>
+        <v>45972</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.6359716520654831</v>
+        <v>0.1340786938261886</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45971</v>
+        <v>45973</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.6260983226885014</v>
+        <v>0.1335983523348238</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45972</v>
+        <v>45974</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.6197587140540662</v>
+        <v>0.1336548873403932</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45973</v>
+        <v>45975</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.6170677713373381</v>
+        <v>0.133654410503235</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45974</v>
+        <v>45978</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.6185438885960699</v>
+        <v>0.1336548426369097</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45975</v>
+        <v>45979</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.6193557328281218</v>
+        <v>0.1329024155868935</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45978</v>
+        <v>45980</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.6195280367346949</v>
+        <v>0.1329026689066338</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45979</v>
+        <v>45981</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>SELL</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.6197502568040014</v>
+        <v>0.1329030563368248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>